<commit_message>
remove site specific from show and index page
</commit_message>
<xml_diff>
--- a/RT database.xlsx
+++ b/RT database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11300" windowHeight="14620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21680" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Response db" sheetId="1" r:id="rId1"/>
@@ -1043,9 +1043,6 @@
     <t>"so let's take care of this matter. "</t>
   </si>
   <si>
-    <t>"We remain commited to you. Please email me at "</t>
-  </si>
-  <si>
     <t>" and let us take care of this. "</t>
   </si>
   <si>
@@ -1067,9 +1064,6 @@
     <t>"Sincerely yours,"</t>
   </si>
   <si>
-    <t>"Commited to excellence in service,"</t>
-  </si>
-  <si>
     <t>"Respectfully at your service,"</t>
   </si>
   <si>
@@ -1094,9 +1088,6 @@
     <t>"Cordial Regards,"</t>
   </si>
   <si>
-    <t>["I look forward to chatting with you and finding a way to resolve your issue.", "Yours,", "Respectfully yours,", "Kindly,", "Looking forward to your call,", "Kindest Regards,", "At your service,", "With my most sincere apologies,", "Sincerely yours,", "Commited to excellence in service,","Respectfully at your service,", "Thanks again for your honest feedback,", "Kind Regards,", "On behalf of our team,"]</t>
-  </si>
-  <si>
     <t>[" Thank you for reaching out to us and letting us know we dropped the ball", "We are truly sorry your experience was not to your satisfaction", "Please allow me to apologize on behalf of everyone here" ,"Thank you for letting us know about this. Feedback helps us tackle issues and become a better business", "We are sad to hear we did not provide you with the best possible experience", "As the person in charge of staffing and customer service I am very dissapointed that we failed you", "Everything that we do is designed to deliver superior customer satisfaction and it appears we have failed you", "On reading your review I cannot help it but feel responsible for having dropped the ball", "Thank you for taking the time to point out personnel issues affecting our business", "It seems we have failed to serve you the way you deserve. That is unacceptable", "We are sad to hear things did not go as expected", "From what we can see your experience was not reflective of our brand. We are really sorry for that", "It saddens me to hear about your experience", "I wanted to personally thank you for taking the time to provide feedback about your experience with us", "It seems we had a disconnect and clearly dropped the ball", "Communications are essential to a good experience and somehow we managed to fail you in this area",  "Thank you for taking the time out of your busy day to let us know about this"]</t>
   </si>
   <si>
@@ -1106,9 +1097,6 @@
     <t>["Our goal is customer satisfaction and we clearly failed to deliver. ", "We are looking into the issue and doing everything we can to correct it as soon as possible, for you and for future customers. ", "We love what we do and we want for every customer to have the best possible experience. ", "Our leadership is trying to identify why this happened and we will resolve in a way that ensures superior customer experiences now and in the future. ", "We are constantly refining the way we do business and that is only possible thanks to candid feedback like yours. Please know that we are listening. ", "Our commitment is to have staff that prioritizes the needs of the customer and is solution-driven every single time. ", "Lack of focus, carelessness and indifference is not what we are known for. We are sorry your experience was not reflective of our reputation. ", "We want to be #1 when it comes to customer service and clearly we are missing the mark.", "We can only address problems if we are aware of how our interactions are affecting the customer experience. ", "Everyone in our organization is familiar with our mission statement which is focused on making certain our customers come first. ", "We are always hard at work to make sure our team delivers on our brand promise and every customer has a positive experience. ", "From the moment you walk into our business it is our responsibility to give you the best possible experience and deliver what we promised. ", "As you probably know we are known for excellence in all that we do. What happened to you was not acceptable by any means and we are looking into it. ", "Clearly we did not deliver as promised. We are very sorry to have failed you. ", "Our staff is aware of your concern and they are looking into ways that similar issues can be avoided in the future. "]</t>
   </si>
   <si>
-    <t>["Please allow us an opportunity to make amends and extend our most sincere apologies. You can contact me directly at  ", "We hope you give us a second chance. Rest assured we won't dissapoint. At your leisure please reach out to us at   ", "We are looking into this issue and hope to resolve it promptly and accurately. ", "We want your business and will do whatever it takes to earn it back. You have our promise. ", "Would you please reach out to me at your leisure via email at ","If you need to contact me to discuss further please reach out to me via email at ", "I can be reached via email at ", "I would like to tackle any issues or concerns that remain unresolved. Please feel free to reach me at ", "We can't fix the past but you have my personal commitment to find ways to improve the way our staff services each and every customer. Please contact me personally via email at ", "Please receive my personal apologies and my invitation to join us. If you have a moment please contact me via email at ", "Thank you for providing honest feedback. Knowing where we are missing the mark helps us tackle our weaknesses as we strive to be better every single day. I am available to discuss this matter at your leisure. Please contact me via email at ", "We know apologies don't fix the past. Please give us a second opportunity to show you what we are truly made of. Please contact me via email at ", "When you have a free moment kindly reach out to me via email at ", "We want you to be satisfied with your transaction. Please contact me at ", "When you have a free moment kindly reach out to me via email at ", " I am ready to help you at any time. You can reach me via phone or by email at ", "We remain commited to you. Please email me at "]</t>
-  </si>
-  <si>
     <t>"Thank you for taking the time to provide us with honest &amp; balanced feedback"</t>
   </si>
   <si>
@@ -1181,21 +1169,12 @@
     <t>"Our commitment is to customer excellence every single transaction. "</t>
   </si>
   <si>
-    <t>"Everyone in our company is commited to the highest levels of quality. "</t>
-  </si>
-  <si>
     <t>"We are sorry this time around we did not deliver as planned. "</t>
   </si>
   <si>
     <t>"Our goal is to deliver customer experiences worth bragging about and this time around we dropped the ball. "</t>
   </si>
   <si>
-    <t>"While your experience was not flawless, we want you to know that we are commited to the highest levels of excellence. "</t>
-  </si>
-  <si>
-    <t>["It looks like we were not up to par in some areas and for that we apologize. "," We have forwarded your concerns to the appropriate departments and will most certainly follow up. ", "Everyone here is open to finding ways to better serve our customers and we will certainly use your insights to develop better business practices. ", "Our commitment is to customer excellence every single transaction. ", "Everyone in our company is commited to the highest levels of quality. ", "We are sorry this time around we did not deliver as planned. ", "We are sorry this time around we did not deliver as planned. ", "Our goal is to deliver customer experiences worth bragging about and this time around we dropped the ball. ", "While your experience was not flawless, we want you to know that we are commited to the highest levels of excellence. ", "While your experience was not flawless, we want you to know that we are commited to the highest levels of excellence. ", ]</t>
-  </si>
-  <si>
     <t>"We are constantly looking for ways to improve our business and it is thanks to feedback like yours that we have made the most impactful changes. "</t>
   </si>
   <si>
@@ -1293,6 +1272,27 @@
   </si>
   <si>
     <t>["With gratitude,", "Respectfully,", "At your service,", "Kindly,", "Yours,", "On behalf of our team,", "Kind Regards,", "With gratitude,"]</t>
+  </si>
+  <si>
+    <t>"We remain committed to you. Please email me at "</t>
+  </si>
+  <si>
+    <t>["Please allow us an opportunity to make amends and extend our most sincere apologies. You can contact me directly at  ", "We hope you give us a second chance. Rest assured we won't dissapoint. At your leisure please reach out to us at   ", "We are looking into this issue and hope to resolve it promptly and accurately. ", "We want your business and will do whatever it takes to earn it back. You have our promise. ", "Would you please reach out to me at your leisure via email at ","If you need to contact me to discuss further please reach out to me via email at ", "I can be reached via email at ", "I would like to tackle any issues or concerns that remain unresolved. Please feel free to reach me at ", "We can't fix the past but you have my personal commitment to find ways to improve the way our staff services each and every customer. Please contact me personally via email at ", "Please receive my personal apologies and my invitation to join us. If you have a moment please contact me via email at ", "Thank you for providing honest feedback. Knowing where we are missing the mark helps us tackle our weaknesses as we strive to be better every single day. I am available to discuss this matter at your leisure. Please contact me via email at ", "We know apologies don't fix the past. Please give us a second opportunity to show you what we are truly made of. Please contact me via email at ", "When you have a free moment kindly reach out to me via email at ", "We want you to be satisfied with your transaction. Please contact me at ", "When you have a free moment kindly reach out to me via email at ", " I am ready to help you at any time. You can reach me via phone or by email at ", "We remain committed to you. Please email me at "]</t>
+  </si>
+  <si>
+    <t>"Everyone in our company is committed to the highest levels of quality. "</t>
+  </si>
+  <si>
+    <t>"While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. "</t>
+  </si>
+  <si>
+    <t>["It looks like we were not up to par in some areas and for that we apologize. "," We have forwarded your concerns to the appropriate departments and will most certainly follow up. ", "Everyone here is open to finding ways to better serve our customers and we will certainly use your insights to develop better business practices. ", "Our commitment is to customer excellence every single transaction. ", "Everyone in our company is committed to the highest levels of quality. ", "We are sorry this time around we did not deliver as planned. ", "We are sorry this time around we did not deliver as planned. ", "Our goal is to deliver customer experiences worth bragging about and this time around we dropped the ball. ", "While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. ", "While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. ", ]</t>
+  </si>
+  <si>
+    <t>"Committed to excellence in service,"</t>
+  </si>
+  <si>
+    <t>["I look forward to chatting with you and finding a way to resolve your issue.", "Yours,", "Respectfully yours,", "Kindly,", "Looking forward to your call,", "Kindest Regards,", "At your service,", "With my most sincere apologies,", "Sincerely yours,", "Committed to excellence in service,","Respectfully at your service,", "Thanks again for your honest feedback,", "Kind Regards,", "On behalf of our team,"]</t>
   </si>
 </sst>
 </file>
@@ -1395,8 +1395,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1567">
+  <cellStyleXfs count="1595">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3016,7 +3044,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1567">
+  <cellStyles count="1595">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3800,6 +3828,20 @@
     <cellStyle name="Followed Hyperlink" xfId="1562" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1564" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1594" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4583,6 +4625,20 @@
     <cellStyle name="Hyperlink" xfId="1561" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1563" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1593" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4914,8 +4970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O49" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="R59" sqref="R59"/>
+    <sheetView tabSelected="1" topLeftCell="H52" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -6105,7 +6161,7 @@
         <v>37</v>
       </c>
       <c r="R29" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="S29" s="5" t="s">
         <v>37</v>
@@ -6155,7 +6211,7 @@
         <v>38</v>
       </c>
       <c r="R30" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S30" s="5" t="s">
         <v>38</v>
@@ -6205,7 +6261,7 @@
         <v>39</v>
       </c>
       <c r="R31" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S31" s="5" t="s">
         <v>39</v>
@@ -6305,7 +6361,7 @@
         <v>41</v>
       </c>
       <c r="R33" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S33" s="5" t="s">
         <v>41</v>
@@ -6452,7 +6508,7 @@
         <v>212</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="S36" s="5" t="s">
         <v>212</v>
@@ -6502,7 +6558,7 @@
         <v>213</v>
       </c>
       <c r="R37" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S37" s="5" t="s">
         <v>213</v>
@@ -6552,7 +6608,7 @@
         <v>214</v>
       </c>
       <c r="R38" s="6" t="s">
-        <v>342</v>
+        <v>416</v>
       </c>
       <c r="S38" s="5" t="s">
         <v>214</v>
@@ -6602,7 +6658,7 @@
         <v>215</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="S39" s="5" t="s">
         <v>215</v>
@@ -6652,7 +6708,7 @@
         <v>216</v>
       </c>
       <c r="R40" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="S40" s="5" t="s">
         <v>216</v>
@@ -6702,7 +6758,7 @@
         <v>217</v>
       </c>
       <c r="R41" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="S41" s="5" t="s">
         <v>217</v>
@@ -6752,7 +6808,7 @@
         <v>218</v>
       </c>
       <c r="R42" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="S42" s="5" t="s">
         <v>218</v>
@@ -6799,7 +6855,7 @@
         <v>219</v>
       </c>
       <c r="R43" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="S43" s="5" t="s">
         <v>219</v>
@@ -6846,7 +6902,7 @@
         <v>220</v>
       </c>
       <c r="R44" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="S44" s="5" t="s">
         <v>220</v>
@@ -6878,13 +6934,13 @@
         <v>221</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>334</v>
+        <v>411</v>
       </c>
       <c r="M45" s="5" t="s">
         <v>221</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="O45" s="5" t="s">
         <v>221</v>
@@ -6893,7 +6949,7 @@
         <v>221</v>
       </c>
       <c r="R45" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="S45" s="5" t="s">
         <v>221</v>
@@ -6928,7 +6984,7 @@
         <v>222</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="S46" s="5" t="s">
         <v>222</v>
@@ -6965,10 +7021,10 @@
     </row>
     <row r="48" spans="3:19" ht="240">
       <c r="D48" s="7" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="H48" s="5" t="s">
         <v>284</v>
@@ -6977,13 +7033,13 @@
         <v>303</v>
       </c>
       <c r="L48" s="5" t="s">
-        <v>355</v>
+        <v>412</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="R48" s="6" t="s">
-        <v>351</v>
+        <v>417</v>
       </c>
     </row>
     <row r="50" spans="1:19" s="11" customFormat="1">
@@ -7053,37 +7109,37 @@
         <v>37</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>37</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>37</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>37</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="K53" s="5" t="s">
         <v>37</v>
       </c>
       <c r="L53" s="5" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="M53" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="O53" s="5" t="s">
         <v>37</v>
@@ -7092,7 +7148,7 @@
         <v>37</v>
       </c>
       <c r="R53" s="6" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="S53" s="5" t="s">
         <v>37</v>
@@ -7103,37 +7159,37 @@
         <v>38</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>38</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>38</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="K54" s="5" t="s">
         <v>38</v>
       </c>
       <c r="L54" s="5" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="M54" s="5" t="s">
         <v>38</v>
       </c>
       <c r="N54" s="2" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="O54" s="5" t="s">
         <v>38</v>
@@ -7153,37 +7209,37 @@
         <v>39</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="K55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="L55" s="5" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="M55" s="5" t="s">
         <v>39</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="O55" s="5" t="s">
         <v>39</v>
@@ -7203,37 +7259,37 @@
         <v>40</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="I56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="K56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="M56" s="5" t="s">
         <v>40</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="O56" s="5" t="s">
         <v>40</v>
@@ -7253,37 +7309,37 @@
         <v>41</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>41</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>41</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>380</v>
+        <v>413</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>41</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="K57" s="5" t="s">
         <v>41</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>41</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="O57" s="5" t="s">
         <v>41</v>
@@ -7292,7 +7348,7 @@
         <v>41</v>
       </c>
       <c r="R57" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S57" s="5" t="s">
         <v>41</v>
@@ -7303,37 +7359,37 @@
         <v>42</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>42</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>42</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="I58" s="5" t="s">
         <v>42</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="K58" s="5" t="s">
         <v>42</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="M58" s="5" t="s">
         <v>42</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="O58" s="5" t="s">
         <v>42</v>
@@ -7342,7 +7398,7 @@
         <v>42</v>
       </c>
       <c r="R58" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="S58" s="5" t="s">
         <v>42</v>
@@ -7353,37 +7409,37 @@
         <v>211</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>211</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>211</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>211</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="K59" s="5" t="s">
         <v>211</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="M59" s="5" t="s">
         <v>211</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="O59" s="5" t="s">
         <v>211</v>
@@ -7392,7 +7448,7 @@
         <v>211</v>
       </c>
       <c r="R59" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="S59" s="5" t="s">
         <v>211</v>
@@ -7403,37 +7459,37 @@
         <v>212</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>212</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>212</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>212</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="K60" s="5" t="s">
         <v>212</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="M60" s="5" t="s">
         <v>212</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="O60" s="5" t="s">
         <v>212</v>
@@ -7442,7 +7498,7 @@
         <v>212</v>
       </c>
       <c r="R60" s="6" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="S60" s="5" t="s">
         <v>212</v>
@@ -7453,37 +7509,37 @@
         <v>213</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>213</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>213</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>383</v>
+        <v>414</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>213</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="K61" s="5" t="s">
         <v>213</v>
       </c>
       <c r="L61" s="5" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="M61" s="5" t="s">
         <v>213</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="O61" s="5" t="s">
         <v>213</v>
@@ -7506,7 +7562,7 @@
         <v>214</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="I62" s="5" t="s">
         <v>214</v>
@@ -7515,7 +7571,7 @@
         <v>214</v>
       </c>
       <c r="L62" s="5" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="M62" s="5" t="s">
         <v>214</v>
@@ -7532,25 +7588,25 @@
     </row>
     <row r="65" spans="1:19" ht="160">
       <c r="D65" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>384</v>
+        <v>415</v>
       </c>
       <c r="J65" s="5" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="L65" s="5" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="R65" s="6" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:19" s="11" customFormat="1" ht="15">

</xml_diff>

<commit_message>
added design files, replaced responses/index with Allie's index, moved images to assets/images
</commit_message>
<xml_diff>
--- a/RT database.xlsx
+++ b/RT database.xlsx
@@ -1250,6 +1250,9 @@
   </si>
   <si>
     <t>"While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. "</t>
+  </si>
+  <si>
+    <t>["It looks like we were not up to par in some areas and for that we apologize. "," We have forwarded your concerns to the appropriate departments and will most certainly follow up. ", "Everyone here is open to finding ways to better serve our customers and we will certainly use your insights to develop better business practices. ", "Our commitment is to customer excellence every single transaction. ", "Everyone in our company is committed to the highest levels of quality. ", "We are sorry this time around we did not deliver as planned. ", "We are sorry this time around we did not deliver as planned. ", "Our goal is to deliver customer experiences worth bragging about and this time around we dropped the ball. ", "While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. ", "While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. ", ]</t>
   </si>
   <si>
     <t>"Committed to excellence in service,"</t>
@@ -1294,9 +1297,6 @@
   </si>
   <si>
     <t>Neutral</t>
-  </si>
-  <si>
-    <t>["It looks like we were not up to par in some areas and for that we apologize. "," We have forwarded your concerns to the appropriate departments and will most certainly follow up. ", "Everyone here is open to finding ways to better serve our customers and we will certainly use your insights to develop better business practices. ", "Our commitment is to customer excellence every single transaction. ", "Everyone in our company is committed to the highest levels of quality. ", "We are sorry this time around we did not deliver as planned. ", "We are sorry this time around we did not deliver as planned. ", "Our goal is to deliver customer experiences worth bragging about and this time around we dropped the ball. ", "While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. ", "While your experience was not flawless, we want you to know that we are committed to the highest levels of excellence. " ]</t>
   </si>
 </sst>
 </file>
@@ -1366,8 +1366,196 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1681">
+  <cellStyleXfs count="1869">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3071,7 +3259,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1681">
+  <cellStyles count="1869">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3912,6 +4100,100 @@
     <cellStyle name="Followed Hyperlink" xfId="1676" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1678" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1680" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1682" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1684" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1686" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1800" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1802" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1804" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1806" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1808" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1810" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1812" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1814" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1816" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1818" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1820" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1822" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1824" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1826" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1828" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1830" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1832" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1834" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1836" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1838" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1840" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1842" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1844" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1846" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1848" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1868" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4752,6 +5034,100 @@
     <cellStyle name="Hyperlink" xfId="1675" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1677" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1679" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1681" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1683" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1685" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1799" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1801" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1803" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1805" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1807" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1809" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1811" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1813" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1815" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1817" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1819" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1821" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1823" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1825" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1827" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1829" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1831" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1833" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1835" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1837" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1839" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1841" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1843" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1845" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1847" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1867" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5083,8 +5459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E49" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="M52" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="R65" sqref="R65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5148,7 +5524,7 @@
         <v>90</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>37</v>
@@ -6165,7 +6541,7 @@
         <v>229</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="27" spans="1:19" s="6" customFormat="1">
@@ -6228,7 +6604,7 @@
         <v>91</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>37</v>
@@ -6720,7 +7096,7 @@
         <v>211</v>
       </c>
       <c r="R38" s="5" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="S38" s="5" t="s">
         <v>211</v>
@@ -7151,7 +7527,7 @@
         <v>346</v>
       </c>
       <c r="R48" s="5" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="50" spans="1:19" s="6" customFormat="1">
@@ -7214,7 +7590,7 @@
         <v>92</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>37</v>
@@ -7705,7 +8081,7 @@
         <v>366</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="J65" s="5" t="s">
         <v>384</v>
@@ -7714,7 +8090,7 @@
         <v>394</v>
       </c>
       <c r="N65" s="5" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="R65" s="5" t="s">
         <v>405</v>

</xml_diff>